<commit_message>
Quest Winds of Fate: A Promise (10752). Contributed by gigilo1968.
</commit_message>
<xml_diff>
--- a/trunk/dist/game/data/scripts/quests/QuestsToDo.xlsx
+++ b/trunk/dist/game/data/scripts/quests/QuestsToDo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="788" uniqueCount="786">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="787" uniqueCount="785">
   <si>
     <t>Parcel Delivery</t>
   </si>
@@ -2195,9 +2195,6 @@
   </si>
   <si>
     <t>https://l2wiki.com/Mysterious_Suggestion_-_2</t>
-  </si>
-  <si>
-    <t>https://l2wiki.com/Winds_of_Fate:_A_Promise</t>
   </si>
   <si>
     <t>https://l2wiki.com/Winds_of_Fate:_Choices</t>
@@ -2750,7 +2747,7 @@
   <dimension ref="A1:E530"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2767,7 +2764,7 @@
         <v>529</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="16.5">
@@ -2778,7 +2775,7 @@
         <v>0</v>
       </c>
       <c r="D2" s="4">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="E2" t="s">
         <v>530</v>
@@ -2793,7 +2790,7 @@
       </c>
       <c r="D3" s="5">
         <f>(D2*100)/529</f>
-        <v>51.984877126654062</v>
+        <v>52.173913043478258</v>
       </c>
       <c r="E3" t="s">
         <v>531</v>
@@ -6964,14 +6961,11 @@
       </c>
     </row>
     <row r="451" spans="1:3">
-      <c r="A451" s="1">
+      <c r="A451" s="3">
         <v>10752</v>
       </c>
-      <c r="B451" s="1" t="s">
+      <c r="B451" s="3" t="s">
         <v>448</v>
-      </c>
-      <c r="C451" t="s">
-        <v>727</v>
       </c>
     </row>
     <row r="452" spans="1:3">
@@ -6982,7 +6976,7 @@
         <v>449</v>
       </c>
       <c r="C452" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
     </row>
     <row r="453" spans="1:3">
@@ -7073,7 +7067,7 @@
         <v>460</v>
       </c>
       <c r="C463" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
     </row>
     <row r="464" spans="1:3">
@@ -7116,7 +7110,7 @@
         <v>465</v>
       </c>
       <c r="C468" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
     </row>
     <row r="469" spans="1:3">
@@ -7135,7 +7129,7 @@
         <v>467</v>
       </c>
       <c r="C470" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
     </row>
     <row r="471" spans="1:3">
@@ -7146,7 +7140,7 @@
         <v>468</v>
       </c>
       <c r="C471" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
     </row>
     <row r="472" spans="1:3">
@@ -7157,7 +7151,7 @@
         <v>469</v>
       </c>
       <c r="C472" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
     </row>
     <row r="473" spans="1:3">
@@ -7168,7 +7162,7 @@
         <v>470</v>
       </c>
       <c r="C473" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
     </row>
     <row r="474" spans="1:3">
@@ -7179,7 +7173,7 @@
         <v>471</v>
       </c>
       <c r="C474" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
     </row>
     <row r="475" spans="1:3">
@@ -7198,7 +7192,7 @@
         <v>473</v>
       </c>
       <c r="C476" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
     </row>
     <row r="477" spans="1:3">
@@ -7209,7 +7203,7 @@
         <v>474</v>
       </c>
       <c r="C477" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
     </row>
     <row r="478" spans="1:3">
@@ -7228,7 +7222,7 @@
         <v>476</v>
       </c>
       <c r="C479" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
     </row>
     <row r="480" spans="1:3">
@@ -7239,7 +7233,7 @@
         <v>477</v>
       </c>
       <c r="C480" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
     </row>
     <row r="481" spans="1:3">
@@ -7282,7 +7276,7 @@
         <v>482</v>
       </c>
       <c r="C485" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="486" spans="1:3">
@@ -7293,7 +7287,7 @@
         <v>483</v>
       </c>
       <c r="C486" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="487" spans="1:3">
@@ -7312,7 +7306,7 @@
         <v>485</v>
       </c>
       <c r="C488" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
     </row>
     <row r="489" spans="1:3">
@@ -7323,7 +7317,7 @@
         <v>486</v>
       </c>
       <c r="C489" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
     </row>
     <row r="490" spans="1:3">
@@ -7334,7 +7328,7 @@
         <v>487</v>
       </c>
       <c r="C490" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
     </row>
     <row r="491" spans="1:3">
@@ -7345,7 +7339,7 @@
         <v>488</v>
       </c>
       <c r="C491" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
     </row>
     <row r="492" spans="1:3">
@@ -7356,7 +7350,7 @@
         <v>489</v>
       </c>
       <c r="C492" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
     </row>
     <row r="493" spans="1:3">
@@ -7367,7 +7361,7 @@
         <v>490</v>
       </c>
       <c r="C493" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
     </row>
     <row r="494" spans="1:3">
@@ -7378,7 +7372,7 @@
         <v>491</v>
       </c>
       <c r="C494" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
     </row>
     <row r="495" spans="1:3">
@@ -7389,7 +7383,7 @@
         <v>492</v>
       </c>
       <c r="C495" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
     </row>
     <row r="496" spans="1:3">
@@ -7400,7 +7394,7 @@
         <v>493</v>
       </c>
       <c r="C496" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
     </row>
     <row r="497" spans="1:3">
@@ -7411,7 +7405,7 @@
         <v>494</v>
       </c>
       <c r="C497" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
     </row>
     <row r="498" spans="1:3">
@@ -7422,7 +7416,7 @@
         <v>495</v>
       </c>
       <c r="C498" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
     </row>
     <row r="499" spans="1:3">
@@ -7433,7 +7427,7 @@
         <v>496</v>
       </c>
       <c r="C499" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
     </row>
     <row r="500" spans="1:3">
@@ -7444,7 +7438,7 @@
         <v>497</v>
       </c>
       <c r="C500" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
     </row>
     <row r="501" spans="1:3">
@@ -7455,7 +7449,7 @@
         <v>498</v>
       </c>
       <c r="C501" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
     </row>
     <row r="502" spans="1:3">
@@ -7466,7 +7460,7 @@
         <v>499</v>
       </c>
       <c r="C502" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
     </row>
     <row r="503" spans="1:3">
@@ -7477,7 +7471,7 @@
         <v>500</v>
       </c>
       <c r="C503" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
     </row>
     <row r="504" spans="1:3">
@@ -7488,7 +7482,7 @@
         <v>501</v>
       </c>
       <c r="C504" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="505" spans="1:3">
@@ -7499,7 +7493,7 @@
         <v>502</v>
       </c>
       <c r="C505" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
     </row>
     <row r="506" spans="1:3">
@@ -7510,7 +7504,7 @@
         <v>503</v>
       </c>
       <c r="C506" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
     </row>
     <row r="507" spans="1:3">
@@ -7521,7 +7515,7 @@
         <v>504</v>
       </c>
       <c r="C507" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
     </row>
     <row r="508" spans="1:3">
@@ -7532,7 +7526,7 @@
         <v>505</v>
       </c>
       <c r="C508" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
     </row>
     <row r="509" spans="1:3">
@@ -7543,7 +7537,7 @@
         <v>506</v>
       </c>
       <c r="C509" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
     </row>
     <row r="510" spans="1:3">
@@ -7554,7 +7548,7 @@
         <v>507</v>
       </c>
       <c r="C510" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
     </row>
     <row r="511" spans="1:3">
@@ -7565,7 +7559,7 @@
         <v>508</v>
       </c>
       <c r="C511" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
     </row>
     <row r="512" spans="1:3">
@@ -7576,7 +7570,7 @@
         <v>509</v>
       </c>
       <c r="C512" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
     </row>
     <row r="513" spans="1:3">
@@ -7587,7 +7581,7 @@
         <v>510</v>
       </c>
       <c r="C513" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
     </row>
     <row r="514" spans="1:3">
@@ -7598,7 +7592,7 @@
         <v>511</v>
       </c>
       <c r="C514" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
     </row>
     <row r="515" spans="1:3">
@@ -7609,7 +7603,7 @@
         <v>512</v>
       </c>
       <c r="C515" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
     </row>
     <row r="516" spans="1:3">
@@ -7620,7 +7614,7 @@
         <v>513</v>
       </c>
       <c r="C516" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
     </row>
     <row r="517" spans="1:3">
@@ -7631,7 +7625,7 @@
         <v>514</v>
       </c>
       <c r="C517" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
     </row>
     <row r="518" spans="1:3">
@@ -7642,7 +7636,7 @@
         <v>515</v>
       </c>
       <c r="C518" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
     </row>
     <row r="519" spans="1:3">
@@ -7653,7 +7647,7 @@
         <v>516</v>
       </c>
       <c r="C519" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
     </row>
     <row r="520" spans="1:3">
@@ -7664,7 +7658,7 @@
         <v>517</v>
       </c>
       <c r="C520" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
     </row>
     <row r="521" spans="1:3">
@@ -7675,7 +7669,7 @@
         <v>518</v>
       </c>
       <c r="C521" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="522" spans="1:3">
@@ -7686,7 +7680,7 @@
         <v>519</v>
       </c>
       <c r="C522" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="523" spans="1:3">
@@ -7697,7 +7691,7 @@
         <v>520</v>
       </c>
       <c r="C523" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
     </row>
     <row r="524" spans="1:3">
@@ -7708,7 +7702,7 @@
         <v>521</v>
       </c>
       <c r="C524" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
     </row>
     <row r="525" spans="1:3">
@@ -7719,7 +7713,7 @@
         <v>522</v>
       </c>
       <c r="C525" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
     </row>
     <row r="526" spans="1:3">
@@ -7730,7 +7724,7 @@
         <v>523</v>
       </c>
       <c r="C526" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
     </row>
     <row r="527" spans="1:3">
@@ -7741,7 +7735,7 @@
         <v>524</v>
       </c>
       <c r="C527" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
     </row>
     <row r="528" spans="1:3">
@@ -7752,7 +7746,7 @@
         <v>525</v>
       </c>
       <c r="C528" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
     </row>
     <row r="529" spans="1:3">
@@ -7763,7 +7757,7 @@
         <v>526</v>
       </c>
       <c r="C529" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
     </row>
     <row r="530" spans="1:3">
@@ -7774,7 +7768,7 @@
         <v>527</v>
       </c>
       <c r="C530" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Quest 1000 years, the End of Lamentation (344).
</commit_message>
<xml_diff>
--- a/trunk/dist/game/data/scripts/quests/QuestsToDo.xlsx
+++ b/trunk/dist/game/data/scripts/quests/QuestsToDo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="787" uniqueCount="785">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="786" uniqueCount="784">
   <si>
     <t>Parcel Delivery</t>
   </si>
@@ -1619,9 +1619,6 @@
   </si>
   <si>
     <t>https://l2wiki.com/Legendary_Tales</t>
-  </si>
-  <si>
-    <t>https://l2wiki.com/1000_years,_the_End_of_Lamentation</t>
   </si>
   <si>
     <t>https://l2wiki.com/Completely_Lost</t>
@@ -2764,7 +2761,7 @@
         <v>529</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="16.5">
@@ -2775,7 +2772,7 @@
         <v>0</v>
       </c>
       <c r="D2" s="4">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="E2" t="s">
         <v>530</v>
@@ -2790,7 +2787,7 @@
       </c>
       <c r="D3" s="5">
         <f>(D2*100)/529</f>
-        <v>52.173913043478258</v>
+        <v>52.362948960302461</v>
       </c>
       <c r="E3" t="s">
         <v>531</v>
@@ -3421,7 +3418,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="81" spans="1:3">
+    <row r="81" spans="1:2">
       <c r="A81" s="3">
         <v>298</v>
       </c>
@@ -3429,7 +3426,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="82" spans="1:3">
+    <row r="82" spans="1:2">
       <c r="A82" s="3">
         <v>307</v>
       </c>
@@ -3437,7 +3434,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="83" spans="1:3">
+    <row r="83" spans="1:2">
       <c r="A83" s="3">
         <v>310</v>
       </c>
@@ -3445,7 +3442,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="84" spans="1:3">
+    <row r="84" spans="1:2">
       <c r="A84" s="3">
         <v>336</v>
       </c>
@@ -3453,7 +3450,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="85" spans="1:3">
+    <row r="85" spans="1:2">
       <c r="A85" s="3">
         <v>337</v>
       </c>
@@ -3461,18 +3458,15 @@
         <v>83</v>
       </c>
     </row>
-    <row r="86" spans="1:3">
-      <c r="A86" s="1">
+    <row r="86" spans="1:2">
+      <c r="A86" s="3">
         <v>344</v>
       </c>
-      <c r="B86" s="1" t="s">
+      <c r="B86" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="C86" t="s">
-        <v>535</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3">
+    </row>
+    <row r="87" spans="1:2">
       <c r="A87" s="3">
         <v>359</v>
       </c>
@@ -3480,7 +3474,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="88" spans="1:3">
+    <row r="88" spans="1:2">
       <c r="A88" s="3">
         <v>371</v>
       </c>
@@ -3488,7 +3482,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="89" spans="1:3">
+    <row r="89" spans="1:2">
       <c r="A89" s="3">
         <v>373</v>
       </c>
@@ -3496,7 +3490,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="90" spans="1:3">
+    <row r="90" spans="1:2">
       <c r="A90" s="3">
         <v>376</v>
       </c>
@@ -3504,7 +3498,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="91" spans="1:3">
+    <row r="91" spans="1:2">
       <c r="A91" s="3">
         <v>377</v>
       </c>
@@ -3512,7 +3506,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="92" spans="1:3">
+    <row r="92" spans="1:2">
       <c r="A92" s="3">
         <v>381</v>
       </c>
@@ -3520,7 +3514,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="93" spans="1:3">
+    <row r="93" spans="1:2">
       <c r="A93" s="3">
         <v>382</v>
       </c>
@@ -3528,7 +3522,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="94" spans="1:3">
+    <row r="94" spans="1:2">
       <c r="A94" s="3">
         <v>386</v>
       </c>
@@ -3536,7 +3530,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="95" spans="1:3">
+    <row r="95" spans="1:2">
       <c r="A95" s="3">
         <v>420</v>
       </c>
@@ -3544,7 +3538,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="96" spans="1:3">
+    <row r="96" spans="1:2">
       <c r="A96" s="3">
         <v>421</v>
       </c>
@@ -3608,7 +3602,7 @@
         <v>101</v>
       </c>
       <c r="C103" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="104" spans="1:3">
@@ -3651,7 +3645,7 @@
         <v>106</v>
       </c>
       <c r="C108" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="109" spans="1:3">
@@ -3662,7 +3656,7 @@
         <v>107</v>
       </c>
       <c r="C109" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="110" spans="1:3">
@@ -3673,7 +3667,7 @@
         <v>108</v>
       </c>
       <c r="C110" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="111" spans="1:3">
@@ -3700,7 +3694,7 @@
         <v>111</v>
       </c>
       <c r="C113" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="114" spans="1:3">
@@ -3711,7 +3705,7 @@
         <v>112</v>
       </c>
       <c r="C114" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="115" spans="1:3">
@@ -3722,7 +3716,7 @@
         <v>113</v>
       </c>
       <c r="C115" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="116" spans="1:3">
@@ -3733,7 +3727,7 @@
         <v>114</v>
       </c>
       <c r="C116" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="117" spans="1:3">
@@ -3776,7 +3770,7 @@
         <v>119</v>
       </c>
       <c r="C121" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="122" spans="1:3">
@@ -3787,7 +3781,7 @@
         <v>120</v>
       </c>
       <c r="C122" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="123" spans="1:3">
@@ -3798,7 +3792,7 @@
         <v>121</v>
       </c>
       <c r="C123" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="124" spans="1:3">
@@ -3809,7 +3803,7 @@
         <v>122</v>
       </c>
       <c r="C124" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="125" spans="1:3">
@@ -3820,7 +3814,7 @@
         <v>123</v>
       </c>
       <c r="C125" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="126" spans="1:3">
@@ -3831,7 +3825,7 @@
         <v>124</v>
       </c>
       <c r="C126" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="127" spans="1:3">
@@ -3874,7 +3868,7 @@
         <v>129</v>
       </c>
       <c r="C131" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="132" spans="1:3">
@@ -3893,7 +3887,7 @@
         <v>131</v>
       </c>
       <c r="C133" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="134" spans="1:3">
@@ -3952,7 +3946,7 @@
         <v>138</v>
       </c>
       <c r="C140" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="141" spans="1:3">
@@ -3987,7 +3981,7 @@
         <v>142</v>
       </c>
       <c r="C144" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="145" spans="1:3">
@@ -4030,7 +4024,7 @@
         <v>147</v>
       </c>
       <c r="C149" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="150" spans="1:3">
@@ -4073,7 +4067,7 @@
         <v>152</v>
       </c>
       <c r="C154" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="155" spans="1:3">
@@ -4212,7 +4206,7 @@
         <v>169</v>
       </c>
       <c r="C171" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="172" spans="1:3">
@@ -4223,7 +4217,7 @@
         <v>170</v>
       </c>
       <c r="C172" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="173" spans="1:3">
@@ -4234,7 +4228,7 @@
         <v>171</v>
       </c>
       <c r="C173" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="174" spans="1:3">
@@ -4245,7 +4239,7 @@
         <v>172</v>
       </c>
       <c r="C174" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="175" spans="1:3">
@@ -4256,7 +4250,7 @@
         <v>173</v>
       </c>
       <c r="C175" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="176" spans="1:3">
@@ -4267,7 +4261,7 @@
         <v>174</v>
       </c>
       <c r="C176" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="177" spans="1:3">
@@ -4278,7 +4272,7 @@
         <v>175</v>
       </c>
       <c r="C177" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="178" spans="1:3">
@@ -4297,7 +4291,7 @@
         <v>177</v>
       </c>
       <c r="C179" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="180" spans="1:3">
@@ -4308,7 +4302,7 @@
         <v>178</v>
       </c>
       <c r="C180" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="181" spans="1:3">
@@ -4319,7 +4313,7 @@
         <v>179</v>
       </c>
       <c r="C181" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="182" spans="1:3">
@@ -4330,7 +4324,7 @@
         <v>180</v>
       </c>
       <c r="C182" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="183" spans="1:3">
@@ -4341,7 +4335,7 @@
         <v>181</v>
       </c>
       <c r="C183" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="184" spans="1:3">
@@ -4352,7 +4346,7 @@
         <v>182</v>
       </c>
       <c r="C184" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="185" spans="1:3">
@@ -4395,7 +4389,7 @@
         <v>187</v>
       </c>
       <c r="C189" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="190" spans="1:3">
@@ -4406,7 +4400,7 @@
         <v>188</v>
       </c>
       <c r="C190" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="191" spans="1:3">
@@ -4425,7 +4419,7 @@
         <v>190</v>
       </c>
       <c r="C192" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="193" spans="1:3">
@@ -4436,7 +4430,7 @@
         <v>191</v>
       </c>
       <c r="C193" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="194" spans="1:3">
@@ -4447,7 +4441,7 @@
         <v>192</v>
       </c>
       <c r="C194" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="195" spans="1:3">
@@ -4458,7 +4452,7 @@
         <v>193</v>
       </c>
       <c r="C195" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="196" spans="1:3">
@@ -4469,7 +4463,7 @@
         <v>194</v>
       </c>
       <c r="C196" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="197" spans="1:3">
@@ -4480,7 +4474,7 @@
         <v>195</v>
       </c>
       <c r="C197" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="198" spans="1:3">
@@ -4491,7 +4485,7 @@
         <v>196</v>
       </c>
       <c r="C198" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="199" spans="1:3">
@@ -4502,7 +4496,7 @@
         <v>197</v>
       </c>
       <c r="C199" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="200" spans="1:3">
@@ -4513,7 +4507,7 @@
         <v>198</v>
       </c>
       <c r="C200" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="201" spans="1:3">
@@ -4524,7 +4518,7 @@
         <v>199</v>
       </c>
       <c r="C201" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="202" spans="1:3">
@@ -4535,7 +4529,7 @@
         <v>200</v>
       </c>
       <c r="C202" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="203" spans="1:3">
@@ -4546,7 +4540,7 @@
         <v>201</v>
       </c>
       <c r="C203" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="204" spans="1:3">
@@ -4557,7 +4551,7 @@
         <v>202</v>
       </c>
       <c r="C204" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="205" spans="1:3">
@@ -4568,7 +4562,7 @@
         <v>203</v>
       </c>
       <c r="C205" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="206" spans="1:3">
@@ -4579,7 +4573,7 @@
         <v>204</v>
       </c>
       <c r="C206" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="207" spans="1:3">
@@ -4590,7 +4584,7 @@
         <v>205</v>
       </c>
       <c r="C207" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="208" spans="1:3">
@@ -4601,7 +4595,7 @@
         <v>206</v>
       </c>
       <c r="C208" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="209" spans="1:3">
@@ -4612,7 +4606,7 @@
         <v>207</v>
       </c>
       <c r="C209" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="210" spans="1:3">
@@ -4623,7 +4617,7 @@
         <v>208</v>
       </c>
       <c r="C210" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="211" spans="1:3">
@@ -4634,7 +4628,7 @@
         <v>209</v>
       </c>
       <c r="C211" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="212" spans="1:3">
@@ -4645,7 +4639,7 @@
         <v>210</v>
       </c>
       <c r="C212" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="213" spans="1:3">
@@ -4656,7 +4650,7 @@
         <v>211</v>
       </c>
       <c r="C213" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="214" spans="1:3">
@@ -4667,7 +4661,7 @@
         <v>212</v>
       </c>
       <c r="C214" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="215" spans="1:3">
@@ -4678,7 +4672,7 @@
         <v>213</v>
       </c>
       <c r="C215" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="216" spans="1:3">
@@ -4689,7 +4683,7 @@
         <v>214</v>
       </c>
       <c r="C216" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="217" spans="1:3">
@@ -4700,7 +4694,7 @@
         <v>215</v>
       </c>
       <c r="C217" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="218" spans="1:3">
@@ -4711,7 +4705,7 @@
         <v>216</v>
       </c>
       <c r="C218" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="219" spans="1:3">
@@ -4722,7 +4716,7 @@
         <v>217</v>
       </c>
       <c r="C219" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="220" spans="1:3">
@@ -4733,7 +4727,7 @@
         <v>218</v>
       </c>
       <c r="C220" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="221" spans="1:3">
@@ -4744,7 +4738,7 @@
         <v>219</v>
       </c>
       <c r="C221" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
     </row>
     <row r="222" spans="1:3">
@@ -4755,7 +4749,7 @@
         <v>220</v>
       </c>
       <c r="C222" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="223" spans="1:3">
@@ -4766,7 +4760,7 @@
         <v>221</v>
       </c>
       <c r="C223" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="224" spans="1:3">
@@ -4777,7 +4771,7 @@
         <v>222</v>
       </c>
       <c r="C224" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
     </row>
     <row r="225" spans="1:3">
@@ -4788,7 +4782,7 @@
         <v>223</v>
       </c>
       <c r="C225" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
     </row>
     <row r="226" spans="1:3">
@@ -4799,7 +4793,7 @@
         <v>224</v>
       </c>
       <c r="C226" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="227" spans="1:3">
@@ -4810,7 +4804,7 @@
         <v>225</v>
       </c>
       <c r="C227" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="228" spans="1:3">
@@ -4821,7 +4815,7 @@
         <v>226</v>
       </c>
       <c r="C228" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
     </row>
     <row r="229" spans="1:3">
@@ -4832,7 +4826,7 @@
         <v>227</v>
       </c>
       <c r="C229" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
     </row>
     <row r="230" spans="1:3">
@@ -4843,7 +4837,7 @@
         <v>228</v>
       </c>
       <c r="C230" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
     </row>
     <row r="231" spans="1:3">
@@ -5062,7 +5056,7 @@
         <v>255</v>
       </c>
       <c r="C257" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
     <row r="258" spans="1:3">
@@ -5073,7 +5067,7 @@
         <v>256</v>
       </c>
       <c r="C258" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="259" spans="1:3">
@@ -5084,7 +5078,7 @@
         <v>257</v>
       </c>
       <c r="C259" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="260" spans="1:3">
@@ -5095,7 +5089,7 @@
         <v>258</v>
       </c>
       <c r="C260" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
     </row>
     <row r="261" spans="1:3">
@@ -5106,7 +5100,7 @@
         <v>259</v>
       </c>
       <c r="C261" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
     </row>
     <row r="262" spans="1:3">
@@ -5117,7 +5111,7 @@
         <v>260</v>
       </c>
       <c r="C262" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
     <row r="263" spans="1:3">
@@ -5128,7 +5122,7 @@
         <v>261</v>
       </c>
       <c r="C263" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
     </row>
     <row r="264" spans="1:3">
@@ -5139,7 +5133,7 @@
         <v>262</v>
       </c>
       <c r="C264" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
     </row>
     <row r="265" spans="1:3">
@@ -5150,7 +5144,7 @@
         <v>263</v>
       </c>
       <c r="C265" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="266" spans="1:3">
@@ -5161,7 +5155,7 @@
         <v>264</v>
       </c>
       <c r="C266" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
     </row>
     <row r="267" spans="1:3">
@@ -5172,7 +5166,7 @@
         <v>265</v>
       </c>
       <c r="C267" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
     </row>
     <row r="268" spans="1:3">
@@ -5183,7 +5177,7 @@
         <v>266</v>
       </c>
       <c r="C268" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
     </row>
     <row r="269" spans="1:3">
@@ -5194,7 +5188,7 @@
         <v>267</v>
       </c>
       <c r="C269" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
     </row>
     <row r="270" spans="1:3">
@@ -5205,7 +5199,7 @@
         <v>268</v>
       </c>
       <c r="C270" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="271" spans="1:3">
@@ -5216,7 +5210,7 @@
         <v>269</v>
       </c>
       <c r="C271" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
     </row>
     <row r="272" spans="1:3">
@@ -5379,7 +5373,7 @@
         <v>289</v>
       </c>
       <c r="C291" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
     </row>
     <row r="292" spans="1:3">
@@ -5438,7 +5432,7 @@
         <v>296</v>
       </c>
       <c r="C298" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
     </row>
     <row r="299" spans="1:3">
@@ -5449,7 +5443,7 @@
         <v>297</v>
       </c>
       <c r="C299" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="300" spans="1:3">
@@ -5460,7 +5454,7 @@
         <v>298</v>
       </c>
       <c r="C300" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
     </row>
     <row r="301" spans="1:3">
@@ -5471,7 +5465,7 @@
         <v>299</v>
       </c>
       <c r="C301" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="302" spans="1:3">
@@ -5482,7 +5476,7 @@
         <v>300</v>
       </c>
       <c r="C302" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
     </row>
     <row r="303" spans="1:3">
@@ -5573,7 +5567,7 @@
         <v>311</v>
       </c>
       <c r="C313" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
     </row>
     <row r="314" spans="1:3">
@@ -5584,7 +5578,7 @@
         <v>312</v>
       </c>
       <c r="C314" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
     </row>
     <row r="315" spans="1:3">
@@ -5595,7 +5589,7 @@
         <v>313</v>
       </c>
       <c r="C315" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
     </row>
     <row r="316" spans="1:3">
@@ -5606,7 +5600,7 @@
         <v>314</v>
       </c>
       <c r="C316" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
     </row>
     <row r="317" spans="1:3">
@@ -5617,7 +5611,7 @@
         <v>315</v>
       </c>
       <c r="C317" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
     </row>
     <row r="318" spans="1:3">
@@ -5628,7 +5622,7 @@
         <v>316</v>
       </c>
       <c r="C318" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
     </row>
     <row r="319" spans="1:3">
@@ -5639,7 +5633,7 @@
         <v>317</v>
       </c>
       <c r="C319" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
     </row>
     <row r="320" spans="1:3">
@@ -5650,7 +5644,7 @@
         <v>318</v>
       </c>
       <c r="C320" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
     </row>
     <row r="321" spans="1:3">
@@ -5661,7 +5655,7 @@
         <v>319</v>
       </c>
       <c r="C321" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
     </row>
     <row r="322" spans="1:3">
@@ -5672,7 +5666,7 @@
         <v>320</v>
       </c>
       <c r="C322" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
     </row>
     <row r="323" spans="1:3">
@@ -5683,7 +5677,7 @@
         <v>321</v>
       </c>
       <c r="C323" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
     </row>
     <row r="324" spans="1:3">
@@ -5742,7 +5736,7 @@
         <v>328</v>
       </c>
       <c r="C330" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
     </row>
     <row r="331" spans="1:3">
@@ -5777,7 +5771,7 @@
         <v>332</v>
       </c>
       <c r="C334" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
     </row>
     <row r="335" spans="1:3">
@@ -5788,7 +5782,7 @@
         <v>333</v>
       </c>
       <c r="C335" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
     </row>
     <row r="336" spans="1:3">
@@ -5807,7 +5801,7 @@
         <v>335</v>
       </c>
       <c r="C337" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
     </row>
     <row r="338" spans="1:3">
@@ -5818,7 +5812,7 @@
         <v>336</v>
       </c>
       <c r="C338" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
     </row>
     <row r="339" spans="1:3">
@@ -5837,7 +5831,7 @@
         <v>338</v>
       </c>
       <c r="C340" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
     </row>
     <row r="341" spans="1:3">
@@ -5848,7 +5842,7 @@
         <v>339</v>
       </c>
       <c r="C341" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
     </row>
     <row r="342" spans="1:3">
@@ -5867,7 +5861,7 @@
         <v>341</v>
       </c>
       <c r="C343" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
     </row>
     <row r="344" spans="1:3">
@@ -5878,7 +5872,7 @@
         <v>342</v>
       </c>
       <c r="C344" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
     </row>
     <row r="345" spans="1:3">
@@ -5897,7 +5891,7 @@
         <v>344</v>
       </c>
       <c r="C346" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="347" spans="1:3">
@@ -5908,7 +5902,7 @@
         <v>345</v>
       </c>
       <c r="C347" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
     </row>
     <row r="348" spans="1:3">
@@ -5927,7 +5921,7 @@
         <v>347</v>
       </c>
       <c r="C349" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="350" spans="1:3">
@@ -5938,7 +5932,7 @@
         <v>348</v>
       </c>
       <c r="C350" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
     </row>
     <row r="351" spans="1:3">
@@ -5957,7 +5951,7 @@
         <v>350</v>
       </c>
       <c r="C352" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
     </row>
     <row r="353" spans="1:3">
@@ -5968,7 +5962,7 @@
         <v>351</v>
       </c>
       <c r="C353" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
     </row>
     <row r="354" spans="1:3">
@@ -5995,7 +5989,7 @@
         <v>354</v>
       </c>
       <c r="C356" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
     </row>
     <row r="357" spans="1:3">
@@ -6006,7 +6000,7 @@
         <v>355</v>
       </c>
       <c r="C357" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
     </row>
     <row r="358" spans="1:3">
@@ -6017,7 +6011,7 @@
         <v>356</v>
       </c>
       <c r="C358" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
     </row>
     <row r="359" spans="1:3">
@@ -6028,7 +6022,7 @@
         <v>357</v>
       </c>
       <c r="C359" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
     </row>
     <row r="360" spans="1:3">
@@ -6039,7 +6033,7 @@
         <v>358</v>
       </c>
       <c r="C360" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="361" spans="1:3">
@@ -6050,7 +6044,7 @@
         <v>359</v>
       </c>
       <c r="C361" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
     </row>
     <row r="362" spans="1:3">
@@ -6061,7 +6055,7 @@
         <v>360</v>
       </c>
       <c r="C362" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
     </row>
     <row r="363" spans="1:3">
@@ -6072,7 +6066,7 @@
         <v>361</v>
       </c>
       <c r="C363" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
     </row>
     <row r="364" spans="1:3">
@@ -6083,7 +6077,7 @@
         <v>362</v>
       </c>
       <c r="C364" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
     </row>
     <row r="365" spans="1:3">
@@ -6094,7 +6088,7 @@
         <v>363</v>
       </c>
       <c r="C365" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="366" spans="1:3">
@@ -6105,7 +6099,7 @@
         <v>364</v>
       </c>
       <c r="C366" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
     </row>
     <row r="367" spans="1:3">
@@ -6116,7 +6110,7 @@
         <v>365</v>
       </c>
       <c r="C367" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
     </row>
     <row r="368" spans="1:3">
@@ -6127,7 +6121,7 @@
         <v>366</v>
       </c>
       <c r="C368" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
     </row>
     <row r="369" spans="1:3">
@@ -6138,7 +6132,7 @@
         <v>367</v>
       </c>
       <c r="C369" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
     </row>
     <row r="370" spans="1:3">
@@ -6149,7 +6143,7 @@
         <v>368</v>
       </c>
       <c r="C370" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
     </row>
     <row r="371" spans="1:3">
@@ -6160,7 +6154,7 @@
         <v>369</v>
       </c>
       <c r="C371" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
     </row>
     <row r="372" spans="1:3">
@@ -6171,7 +6165,7 @@
         <v>370</v>
       </c>
       <c r="C372" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
     </row>
     <row r="373" spans="1:3">
@@ -6182,7 +6176,7 @@
         <v>371</v>
       </c>
       <c r="C373" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
     </row>
     <row r="374" spans="1:3">
@@ -6193,7 +6187,7 @@
         <v>372</v>
       </c>
       <c r="C374" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
     </row>
     <row r="375" spans="1:3">
@@ -6204,7 +6198,7 @@
         <v>373</v>
       </c>
       <c r="C375" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
     </row>
     <row r="376" spans="1:3">
@@ -6215,7 +6209,7 @@
         <v>374</v>
       </c>
       <c r="C376" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
     </row>
     <row r="377" spans="1:3">
@@ -6226,7 +6220,7 @@
         <v>375</v>
       </c>
       <c r="C377" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
     </row>
     <row r="378" spans="1:3">
@@ -6237,7 +6231,7 @@
         <v>376</v>
       </c>
       <c r="C378" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
     </row>
     <row r="379" spans="1:3">
@@ -6248,7 +6242,7 @@
         <v>377</v>
       </c>
       <c r="C379" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
     </row>
     <row r="380" spans="1:3">
@@ -6259,7 +6253,7 @@
         <v>378</v>
       </c>
       <c r="C380" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
     </row>
     <row r="381" spans="1:3">
@@ -6270,7 +6264,7 @@
         <v>379</v>
       </c>
       <c r="C381" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="382" spans="1:3">
@@ -6281,7 +6275,7 @@
         <v>380</v>
       </c>
       <c r="C382" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
     </row>
     <row r="383" spans="1:3">
@@ -6292,7 +6286,7 @@
         <v>381</v>
       </c>
       <c r="C383" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
     </row>
     <row r="384" spans="1:3">
@@ -6303,7 +6297,7 @@
         <v>382</v>
       </c>
       <c r="C384" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
     </row>
     <row r="385" spans="1:3">
@@ -6314,7 +6308,7 @@
         <v>383</v>
       </c>
       <c r="C385" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
     </row>
     <row r="386" spans="1:3">
@@ -6333,7 +6327,7 @@
         <v>385</v>
       </c>
       <c r="C387" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="388" spans="1:3">
@@ -6344,7 +6338,7 @@
         <v>386</v>
       </c>
       <c r="C388" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
     </row>
     <row r="389" spans="1:3">
@@ -6355,7 +6349,7 @@
         <v>387</v>
       </c>
       <c r="C389" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="390" spans="1:3">
@@ -6366,7 +6360,7 @@
         <v>388</v>
       </c>
       <c r="C390" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="391" spans="1:3">
@@ -6377,7 +6371,7 @@
         <v>389</v>
       </c>
       <c r="C391" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
     </row>
     <row r="392" spans="1:3">
@@ -6388,7 +6382,7 @@
         <v>390</v>
       </c>
       <c r="C392" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
     </row>
     <row r="393" spans="1:3">
@@ -6399,7 +6393,7 @@
         <v>391</v>
       </c>
       <c r="C393" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
     </row>
     <row r="394" spans="1:3">
@@ -6410,7 +6404,7 @@
         <v>392</v>
       </c>
       <c r="C394" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
     </row>
     <row r="395" spans="1:3">
@@ -6421,7 +6415,7 @@
         <v>393</v>
       </c>
       <c r="C395" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
     </row>
     <row r="396" spans="1:3">
@@ -6488,7 +6482,7 @@
         <v>401</v>
       </c>
       <c r="C403" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
     </row>
     <row r="404" spans="1:3">
@@ -6499,7 +6493,7 @@
         <v>402</v>
       </c>
       <c r="C404" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
     </row>
     <row r="405" spans="1:3">
@@ -6510,7 +6504,7 @@
         <v>403</v>
       </c>
       <c r="C405" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
     </row>
     <row r="406" spans="1:3">
@@ -6521,7 +6515,7 @@
         <v>404</v>
       </c>
       <c r="C406" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="407" spans="1:3">
@@ -6532,7 +6526,7 @@
         <v>405</v>
       </c>
       <c r="C407" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
     </row>
     <row r="408" spans="1:3">
@@ -6543,7 +6537,7 @@
         <v>406</v>
       </c>
       <c r="C408" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
     </row>
     <row r="409" spans="1:3">
@@ -6554,7 +6548,7 @@
         <v>407</v>
       </c>
       <c r="C409" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
     </row>
     <row r="410" spans="1:3">
@@ -6565,7 +6559,7 @@
         <v>408</v>
       </c>
       <c r="C410" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
     </row>
     <row r="411" spans="1:3">
@@ -6576,7 +6570,7 @@
         <v>409</v>
       </c>
       <c r="C411" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
     </row>
     <row r="412" spans="1:3">
@@ -6587,7 +6581,7 @@
         <v>410</v>
       </c>
       <c r="C412" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
     </row>
     <row r="413" spans="1:3">
@@ -6598,7 +6592,7 @@
         <v>411</v>
       </c>
       <c r="C413" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="414" spans="1:3">
@@ -6609,7 +6603,7 @@
         <v>412</v>
       </c>
       <c r="C414" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
     </row>
     <row r="415" spans="1:3">
@@ -6620,7 +6614,7 @@
         <v>413</v>
       </c>
       <c r="C415" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
     </row>
     <row r="416" spans="1:3">
@@ -6631,7 +6625,7 @@
         <v>414</v>
       </c>
       <c r="C416" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
     </row>
     <row r="417" spans="1:3">
@@ -6642,7 +6636,7 @@
         <v>415</v>
       </c>
       <c r="C417" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="418" spans="1:3">
@@ -6653,7 +6647,7 @@
         <v>416</v>
       </c>
       <c r="C418" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
     </row>
     <row r="419" spans="1:3">
@@ -6664,7 +6658,7 @@
         <v>417</v>
       </c>
       <c r="C419" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
     </row>
     <row r="420" spans="1:3">
@@ -6675,7 +6669,7 @@
         <v>418</v>
       </c>
       <c r="C420" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
     </row>
     <row r="421" spans="1:3">
@@ -6686,7 +6680,7 @@
         <v>419</v>
       </c>
       <c r="C421" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
     </row>
     <row r="422" spans="1:3">
@@ -6697,7 +6691,7 @@
         <v>420</v>
       </c>
       <c r="C422" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
     </row>
     <row r="423" spans="1:3">
@@ -6708,7 +6702,7 @@
         <v>421</v>
       </c>
       <c r="C423" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
     </row>
     <row r="424" spans="1:3">
@@ -6719,7 +6713,7 @@
         <v>422</v>
       </c>
       <c r="C424" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
     </row>
     <row r="425" spans="1:3">
@@ -6730,7 +6724,7 @@
         <v>423</v>
       </c>
       <c r="C425" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
     </row>
     <row r="426" spans="1:3">
@@ -6741,7 +6735,7 @@
         <v>424</v>
       </c>
       <c r="C426" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
     </row>
     <row r="427" spans="1:3">
@@ -6752,7 +6746,7 @@
         <v>425</v>
       </c>
       <c r="C427" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
     </row>
     <row r="428" spans="1:3">
@@ -6763,7 +6757,7 @@
         <v>426</v>
       </c>
       <c r="C428" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
     </row>
     <row r="429" spans="1:3">
@@ -6774,7 +6768,7 @@
         <v>427</v>
       </c>
       <c r="C429" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
     </row>
     <row r="430" spans="1:3">
@@ -6785,7 +6779,7 @@
         <v>428</v>
       </c>
       <c r="C430" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
     </row>
     <row r="431" spans="1:3">
@@ -6796,7 +6790,7 @@
         <v>429</v>
       </c>
       <c r="C431" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
     </row>
     <row r="432" spans="1:3">
@@ -6927,7 +6921,7 @@
         <v>444</v>
       </c>
       <c r="C447" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
     </row>
     <row r="448" spans="1:3">
@@ -6938,7 +6932,7 @@
         <v>445</v>
       </c>
       <c r="C448" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
     </row>
     <row r="449" spans="1:3">
@@ -6949,7 +6943,7 @@
         <v>446</v>
       </c>
       <c r="C449" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
     </row>
     <row r="450" spans="1:3">
@@ -6976,7 +6970,7 @@
         <v>449</v>
       </c>
       <c r="C452" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
     </row>
     <row r="453" spans="1:3">
@@ -7067,7 +7061,7 @@
         <v>460</v>
       </c>
       <c r="C463" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
     </row>
     <row r="464" spans="1:3">
@@ -7110,7 +7104,7 @@
         <v>465</v>
       </c>
       <c r="C468" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
     </row>
     <row r="469" spans="1:3">
@@ -7129,7 +7123,7 @@
         <v>467</v>
       </c>
       <c r="C470" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
     </row>
     <row r="471" spans="1:3">
@@ -7140,7 +7134,7 @@
         <v>468</v>
       </c>
       <c r="C471" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
     </row>
     <row r="472" spans="1:3">
@@ -7151,7 +7145,7 @@
         <v>469</v>
       </c>
       <c r="C472" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
     </row>
     <row r="473" spans="1:3">
@@ -7162,7 +7156,7 @@
         <v>470</v>
       </c>
       <c r="C473" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
     </row>
     <row r="474" spans="1:3">
@@ -7173,7 +7167,7 @@
         <v>471</v>
       </c>
       <c r="C474" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
     </row>
     <row r="475" spans="1:3">
@@ -7192,7 +7186,7 @@
         <v>473</v>
       </c>
       <c r="C476" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
     </row>
     <row r="477" spans="1:3">
@@ -7203,7 +7197,7 @@
         <v>474</v>
       </c>
       <c r="C477" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
     </row>
     <row r="478" spans="1:3">
@@ -7222,7 +7216,7 @@
         <v>476</v>
       </c>
       <c r="C479" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
     </row>
     <row r="480" spans="1:3">
@@ -7233,7 +7227,7 @@
         <v>477</v>
       </c>
       <c r="C480" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
     </row>
     <row r="481" spans="1:3">
@@ -7276,7 +7270,7 @@
         <v>482</v>
       </c>
       <c r="C485" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
     </row>
     <row r="486" spans="1:3">
@@ -7287,7 +7281,7 @@
         <v>483</v>
       </c>
       <c r="C486" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="487" spans="1:3">
@@ -7306,7 +7300,7 @@
         <v>485</v>
       </c>
       <c r="C488" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="489" spans="1:3">
@@ -7317,7 +7311,7 @@
         <v>486</v>
       </c>
       <c r="C489" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
     </row>
     <row r="490" spans="1:3">
@@ -7328,7 +7322,7 @@
         <v>487</v>
       </c>
       <c r="C490" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
     </row>
     <row r="491" spans="1:3">
@@ -7339,7 +7333,7 @@
         <v>488</v>
       </c>
       <c r="C491" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
     </row>
     <row r="492" spans="1:3">
@@ -7350,7 +7344,7 @@
         <v>489</v>
       </c>
       <c r="C492" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
     </row>
     <row r="493" spans="1:3">
@@ -7361,7 +7355,7 @@
         <v>490</v>
       </c>
       <c r="C493" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
     </row>
     <row r="494" spans="1:3">
@@ -7372,7 +7366,7 @@
         <v>491</v>
       </c>
       <c r="C494" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
     </row>
     <row r="495" spans="1:3">
@@ -7383,7 +7377,7 @@
         <v>492</v>
       </c>
       <c r="C495" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
     </row>
     <row r="496" spans="1:3">
@@ -7394,7 +7388,7 @@
         <v>493</v>
       </c>
       <c r="C496" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
     </row>
     <row r="497" spans="1:3">
@@ -7405,7 +7399,7 @@
         <v>494</v>
       </c>
       <c r="C497" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
     </row>
     <row r="498" spans="1:3">
@@ -7416,7 +7410,7 @@
         <v>495</v>
       </c>
       <c r="C498" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
     </row>
     <row r="499" spans="1:3">
@@ -7427,7 +7421,7 @@
         <v>496</v>
       </c>
       <c r="C499" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
     </row>
     <row r="500" spans="1:3">
@@ -7438,7 +7432,7 @@
         <v>497</v>
       </c>
       <c r="C500" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
     </row>
     <row r="501" spans="1:3">
@@ -7449,7 +7443,7 @@
         <v>498</v>
       </c>
       <c r="C501" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
     </row>
     <row r="502" spans="1:3">
@@ -7460,7 +7454,7 @@
         <v>499</v>
       </c>
       <c r="C502" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
     </row>
     <row r="503" spans="1:3">
@@ -7471,7 +7465,7 @@
         <v>500</v>
       </c>
       <c r="C503" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
     </row>
     <row r="504" spans="1:3">
@@ -7482,7 +7476,7 @@
         <v>501</v>
       </c>
       <c r="C504" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
     </row>
     <row r="505" spans="1:3">
@@ -7493,7 +7487,7 @@
         <v>502</v>
       </c>
       <c r="C505" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="506" spans="1:3">
@@ -7504,7 +7498,7 @@
         <v>503</v>
       </c>
       <c r="C506" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
     </row>
     <row r="507" spans="1:3">
@@ -7515,7 +7509,7 @@
         <v>504</v>
       </c>
       <c r="C507" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
     </row>
     <row r="508" spans="1:3">
@@ -7526,7 +7520,7 @@
         <v>505</v>
       </c>
       <c r="C508" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
     </row>
     <row r="509" spans="1:3">
@@ -7537,7 +7531,7 @@
         <v>506</v>
       </c>
       <c r="C509" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
     </row>
     <row r="510" spans="1:3">
@@ -7548,7 +7542,7 @@
         <v>507</v>
       </c>
       <c r="C510" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
     </row>
     <row r="511" spans="1:3">
@@ -7559,7 +7553,7 @@
         <v>508</v>
       </c>
       <c r="C511" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
     </row>
     <row r="512" spans="1:3">
@@ -7570,7 +7564,7 @@
         <v>509</v>
       </c>
       <c r="C512" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
     </row>
     <row r="513" spans="1:3">
@@ -7581,7 +7575,7 @@
         <v>510</v>
       </c>
       <c r="C513" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
     </row>
     <row r="514" spans="1:3">
@@ -7592,7 +7586,7 @@
         <v>511</v>
       </c>
       <c r="C514" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
     </row>
     <row r="515" spans="1:3">
@@ -7603,7 +7597,7 @@
         <v>512</v>
       </c>
       <c r="C515" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
     </row>
     <row r="516" spans="1:3">
@@ -7614,7 +7608,7 @@
         <v>513</v>
       </c>
       <c r="C516" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
     </row>
     <row r="517" spans="1:3">
@@ -7625,7 +7619,7 @@
         <v>514</v>
       </c>
       <c r="C517" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
     </row>
     <row r="518" spans="1:3">
@@ -7636,7 +7630,7 @@
         <v>515</v>
       </c>
       <c r="C518" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
     </row>
     <row r="519" spans="1:3">
@@ -7647,7 +7641,7 @@
         <v>516</v>
       </c>
       <c r="C519" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
     </row>
     <row r="520" spans="1:3">
@@ -7658,7 +7652,7 @@
         <v>517</v>
       </c>
       <c r="C520" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
     </row>
     <row r="521" spans="1:3">
@@ -7669,7 +7663,7 @@
         <v>518</v>
       </c>
       <c r="C521" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
     </row>
     <row r="522" spans="1:3">
@@ -7680,7 +7674,7 @@
         <v>519</v>
       </c>
       <c r="C522" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="523" spans="1:3">
@@ -7691,7 +7685,7 @@
         <v>520</v>
       </c>
       <c r="C523" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="524" spans="1:3">
@@ -7702,7 +7696,7 @@
         <v>521</v>
       </c>
       <c r="C524" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
     </row>
     <row r="525" spans="1:3">
@@ -7713,7 +7707,7 @@
         <v>522</v>
       </c>
       <c r="C525" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
     </row>
     <row r="526" spans="1:3">
@@ -7724,7 +7718,7 @@
         <v>523</v>
       </c>
       <c r="C526" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
     </row>
     <row r="527" spans="1:3">
@@ -7735,7 +7729,7 @@
         <v>524</v>
       </c>
       <c r="C527" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
     </row>
     <row r="528" spans="1:3">
@@ -7746,7 +7740,7 @@
         <v>525</v>
       </c>
       <c r="C528" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
     </row>
     <row r="529" spans="1:3">
@@ -7757,7 +7751,7 @@
         <v>526</v>
       </c>
       <c r="C529" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
     </row>
     <row r="530" spans="1:3">
@@ -7768,7 +7762,7 @@
         <v>527</v>
       </c>
       <c r="C530" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Quest Letters from the Queen: Dragon Valley (10798). Contributed by gigilo1968.
</commit_message>
<xml_diff>
--- a/trunk/dist/game/data/scripts/quests/QuestsToDo.xlsx
+++ b/trunk/dist/game/data/scripts/quests/QuestsToDo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="786" uniqueCount="784">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="785" uniqueCount="783">
   <si>
     <t>Parcel Delivery</t>
   </si>
@@ -2240,9 +2240,6 @@
   </si>
   <si>
     <t>https://l2wiki.com/Crossing_Fate</t>
-  </si>
-  <si>
-    <t>https://l2wiki.com/Letters_from_the_Queen:_Dragon_Valley</t>
   </si>
   <si>
     <t>https://l2wiki.com/Strange_Things_Afoot_in_the_Valley</t>
@@ -2761,7 +2758,7 @@
         <v>529</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="16.5">
@@ -2772,7 +2769,7 @@
         <v>0</v>
       </c>
       <c r="D2" s="4">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="E2" t="s">
         <v>530</v>
@@ -2787,7 +2784,7 @@
       </c>
       <c r="D3" s="5">
         <f>(D2*100)/529</f>
-        <v>52.362948960302461</v>
+        <v>52.551984877126657</v>
       </c>
       <c r="E3" t="s">
         <v>531</v>
@@ -7315,14 +7312,11 @@
       </c>
     </row>
     <row r="490" spans="1:3">
-      <c r="A490" s="1">
+      <c r="A490" s="3">
         <v>10798</v>
       </c>
-      <c r="B490" s="1" t="s">
+      <c r="B490" s="3" t="s">
         <v>487</v>
-      </c>
-      <c r="C490" t="s">
-        <v>742</v>
       </c>
     </row>
     <row r="491" spans="1:3">
@@ -7333,7 +7327,7 @@
         <v>488</v>
       </c>
       <c r="C491" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
     </row>
     <row r="492" spans="1:3">
@@ -7344,7 +7338,7 @@
         <v>489</v>
       </c>
       <c r="C492" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
     </row>
     <row r="493" spans="1:3">
@@ -7355,7 +7349,7 @@
         <v>490</v>
       </c>
       <c r="C493" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
     </row>
     <row r="494" spans="1:3">
@@ -7366,7 +7360,7 @@
         <v>491</v>
       </c>
       <c r="C494" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
     </row>
     <row r="495" spans="1:3">
@@ -7377,7 +7371,7 @@
         <v>492</v>
       </c>
       <c r="C495" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
     </row>
     <row r="496" spans="1:3">
@@ -7388,7 +7382,7 @@
         <v>493</v>
       </c>
       <c r="C496" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
     </row>
     <row r="497" spans="1:3">
@@ -7399,7 +7393,7 @@
         <v>494</v>
       </c>
       <c r="C497" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
     </row>
     <row r="498" spans="1:3">
@@ -7410,7 +7404,7 @@
         <v>495</v>
       </c>
       <c r="C498" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
     </row>
     <row r="499" spans="1:3">
@@ -7421,7 +7415,7 @@
         <v>496</v>
       </c>
       <c r="C499" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
     </row>
     <row r="500" spans="1:3">
@@ -7432,7 +7426,7 @@
         <v>497</v>
       </c>
       <c r="C500" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
     </row>
     <row r="501" spans="1:3">
@@ -7443,7 +7437,7 @@
         <v>498</v>
       </c>
       <c r="C501" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
     </row>
     <row r="502" spans="1:3">
@@ -7454,7 +7448,7 @@
         <v>499</v>
       </c>
       <c r="C502" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
     </row>
     <row r="503" spans="1:3">
@@ -7465,7 +7459,7 @@
         <v>500</v>
       </c>
       <c r="C503" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
     </row>
     <row r="504" spans="1:3">
@@ -7476,7 +7470,7 @@
         <v>501</v>
       </c>
       <c r="C504" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
     </row>
     <row r="505" spans="1:3">
@@ -7487,7 +7481,7 @@
         <v>502</v>
       </c>
       <c r="C505" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
     </row>
     <row r="506" spans="1:3">
@@ -7498,7 +7492,7 @@
         <v>503</v>
       </c>
       <c r="C506" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="507" spans="1:3">
@@ -7509,7 +7503,7 @@
         <v>504</v>
       </c>
       <c r="C507" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
     </row>
     <row r="508" spans="1:3">
@@ -7520,7 +7514,7 @@
         <v>505</v>
       </c>
       <c r="C508" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
     </row>
     <row r="509" spans="1:3">
@@ -7531,7 +7525,7 @@
         <v>506</v>
       </c>
       <c r="C509" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
     </row>
     <row r="510" spans="1:3">
@@ -7542,7 +7536,7 @@
         <v>507</v>
       </c>
       <c r="C510" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
     </row>
     <row r="511" spans="1:3">
@@ -7553,7 +7547,7 @@
         <v>508</v>
       </c>
       <c r="C511" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
     </row>
     <row r="512" spans="1:3">
@@ -7564,7 +7558,7 @@
         <v>509</v>
       </c>
       <c r="C512" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
     </row>
     <row r="513" spans="1:3">
@@ -7575,7 +7569,7 @@
         <v>510</v>
       </c>
       <c r="C513" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
     </row>
     <row r="514" spans="1:3">
@@ -7586,7 +7580,7 @@
         <v>511</v>
       </c>
       <c r="C514" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
     </row>
     <row r="515" spans="1:3">
@@ -7597,7 +7591,7 @@
         <v>512</v>
       </c>
       <c r="C515" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
     </row>
     <row r="516" spans="1:3">
@@ -7608,7 +7602,7 @@
         <v>513</v>
       </c>
       <c r="C516" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
     </row>
     <row r="517" spans="1:3">
@@ -7619,7 +7613,7 @@
         <v>514</v>
       </c>
       <c r="C517" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
     </row>
     <row r="518" spans="1:3">
@@ -7630,7 +7624,7 @@
         <v>515</v>
       </c>
       <c r="C518" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
     </row>
     <row r="519" spans="1:3">
@@ -7641,7 +7635,7 @@
         <v>516</v>
       </c>
       <c r="C519" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
     </row>
     <row r="520" spans="1:3">
@@ -7652,7 +7646,7 @@
         <v>517</v>
       </c>
       <c r="C520" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
     </row>
     <row r="521" spans="1:3">
@@ -7663,7 +7657,7 @@
         <v>518</v>
       </c>
       <c r="C521" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
     </row>
     <row r="522" spans="1:3">
@@ -7674,7 +7668,7 @@
         <v>519</v>
       </c>
       <c r="C522" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
     </row>
     <row r="523" spans="1:3">
@@ -7685,7 +7679,7 @@
         <v>520</v>
       </c>
       <c r="C523" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="524" spans="1:3">
@@ -7696,7 +7690,7 @@
         <v>521</v>
       </c>
       <c r="C524" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="525" spans="1:3">
@@ -7707,7 +7701,7 @@
         <v>522</v>
       </c>
       <c r="C525" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
     </row>
     <row r="526" spans="1:3">
@@ -7718,7 +7712,7 @@
         <v>523</v>
       </c>
       <c r="C526" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
     </row>
     <row r="527" spans="1:3">
@@ -7729,7 +7723,7 @@
         <v>524</v>
       </c>
       <c r="C527" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
     </row>
     <row r="528" spans="1:3">
@@ -7740,7 +7734,7 @@
         <v>525</v>
       </c>
       <c r="C528" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
     </row>
     <row r="529" spans="1:3">
@@ -7751,7 +7745,7 @@
         <v>526</v>
       </c>
       <c r="C529" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
     </row>
     <row r="530" spans="1:3">
@@ -7762,7 +7756,7 @@
         <v>527</v>
       </c>
       <c r="C530" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Quest Strange Things Afoot in the Valley (10799). Contributed by gigilo1968.
</commit_message>
<xml_diff>
--- a/trunk/dist/game/data/scripts/quests/QuestsToDo.xlsx
+++ b/trunk/dist/game/data/scripts/quests/QuestsToDo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="785" uniqueCount="783">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="784" uniqueCount="782">
   <si>
     <t>Parcel Delivery</t>
   </si>
@@ -2240,9 +2240,6 @@
   </si>
   <si>
     <t>https://l2wiki.com/Crossing_Fate</t>
-  </si>
-  <si>
-    <t>https://l2wiki.com/Strange_Things_Afoot_in_the_Valley</t>
   </si>
   <si>
     <t>https://l2wiki.com/Reconnaissance_at_Dragon_Valley</t>
@@ -2758,7 +2755,7 @@
         <v>529</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="16.5">
@@ -2769,7 +2766,7 @@
         <v>0</v>
       </c>
       <c r="D2" s="4">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="E2" t="s">
         <v>530</v>
@@ -2784,7 +2781,7 @@
       </c>
       <c r="D3" s="5">
         <f>(D2*100)/529</f>
-        <v>52.551984877126657</v>
+        <v>52.741020793950852</v>
       </c>
       <c r="E3" t="s">
         <v>531</v>
@@ -7320,14 +7317,11 @@
       </c>
     </row>
     <row r="491" spans="1:3">
-      <c r="A491" s="1">
+      <c r="A491" s="3">
         <v>10799</v>
       </c>
-      <c r="B491" s="1" t="s">
+      <c r="B491" s="3" t="s">
         <v>488</v>
-      </c>
-      <c r="C491" t="s">
-        <v>742</v>
       </c>
     </row>
     <row r="492" spans="1:3">
@@ -7338,7 +7332,7 @@
         <v>489</v>
       </c>
       <c r="C492" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
     </row>
     <row r="493" spans="1:3">
@@ -7349,7 +7343,7 @@
         <v>490</v>
       </c>
       <c r="C493" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
     </row>
     <row r="494" spans="1:3">
@@ -7360,7 +7354,7 @@
         <v>491</v>
       </c>
       <c r="C494" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
     </row>
     <row r="495" spans="1:3">
@@ -7371,7 +7365,7 @@
         <v>492</v>
       </c>
       <c r="C495" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
     </row>
     <row r="496" spans="1:3">
@@ -7382,7 +7376,7 @@
         <v>493</v>
       </c>
       <c r="C496" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
     </row>
     <row r="497" spans="1:3">
@@ -7393,7 +7387,7 @@
         <v>494</v>
       </c>
       <c r="C497" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
     </row>
     <row r="498" spans="1:3">
@@ -7404,7 +7398,7 @@
         <v>495</v>
       </c>
       <c r="C498" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
     </row>
     <row r="499" spans="1:3">
@@ -7415,7 +7409,7 @@
         <v>496</v>
       </c>
       <c r="C499" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
     </row>
     <row r="500" spans="1:3">
@@ -7426,7 +7420,7 @@
         <v>497</v>
       </c>
       <c r="C500" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
     </row>
     <row r="501" spans="1:3">
@@ -7437,7 +7431,7 @@
         <v>498</v>
       </c>
       <c r="C501" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
     </row>
     <row r="502" spans="1:3">
@@ -7448,7 +7442,7 @@
         <v>499</v>
       </c>
       <c r="C502" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
     </row>
     <row r="503" spans="1:3">
@@ -7459,7 +7453,7 @@
         <v>500</v>
       </c>
       <c r="C503" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
     </row>
     <row r="504" spans="1:3">
@@ -7470,7 +7464,7 @@
         <v>501</v>
       </c>
       <c r="C504" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
     </row>
     <row r="505" spans="1:3">
@@ -7481,7 +7475,7 @@
         <v>502</v>
       </c>
       <c r="C505" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
     </row>
     <row r="506" spans="1:3">
@@ -7492,7 +7486,7 @@
         <v>503</v>
       </c>
       <c r="C506" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
     </row>
     <row r="507" spans="1:3">
@@ -7503,7 +7497,7 @@
         <v>504</v>
       </c>
       <c r="C507" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="508" spans="1:3">
@@ -7514,7 +7508,7 @@
         <v>505</v>
       </c>
       <c r="C508" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
     </row>
     <row r="509" spans="1:3">
@@ -7525,7 +7519,7 @@
         <v>506</v>
       </c>
       <c r="C509" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
     </row>
     <row r="510" spans="1:3">
@@ -7536,7 +7530,7 @@
         <v>507</v>
       </c>
       <c r="C510" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
     </row>
     <row r="511" spans="1:3">
@@ -7547,7 +7541,7 @@
         <v>508</v>
       </c>
       <c r="C511" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
     </row>
     <row r="512" spans="1:3">
@@ -7558,7 +7552,7 @@
         <v>509</v>
       </c>
       <c r="C512" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
     </row>
     <row r="513" spans="1:3">
@@ -7569,7 +7563,7 @@
         <v>510</v>
       </c>
       <c r="C513" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
     </row>
     <row r="514" spans="1:3">
@@ -7580,7 +7574,7 @@
         <v>511</v>
       </c>
       <c r="C514" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
     </row>
     <row r="515" spans="1:3">
@@ -7591,7 +7585,7 @@
         <v>512</v>
       </c>
       <c r="C515" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
     </row>
     <row r="516" spans="1:3">
@@ -7602,7 +7596,7 @@
         <v>513</v>
       </c>
       <c r="C516" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
     </row>
     <row r="517" spans="1:3">
@@ -7613,7 +7607,7 @@
         <v>514</v>
       </c>
       <c r="C517" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
     </row>
     <row r="518" spans="1:3">
@@ -7624,7 +7618,7 @@
         <v>515</v>
       </c>
       <c r="C518" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
     </row>
     <row r="519" spans="1:3">
@@ -7635,7 +7629,7 @@
         <v>516</v>
       </c>
       <c r="C519" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
     </row>
     <row r="520" spans="1:3">
@@ -7646,7 +7640,7 @@
         <v>517</v>
       </c>
       <c r="C520" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
     </row>
     <row r="521" spans="1:3">
@@ -7657,7 +7651,7 @@
         <v>518</v>
       </c>
       <c r="C521" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
     </row>
     <row r="522" spans="1:3">
@@ -7668,7 +7662,7 @@
         <v>519</v>
       </c>
       <c r="C522" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
     </row>
     <row r="523" spans="1:3">
@@ -7679,7 +7673,7 @@
         <v>520</v>
       </c>
       <c r="C523" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
     </row>
     <row r="524" spans="1:3">
@@ -7690,7 +7684,7 @@
         <v>521</v>
       </c>
       <c r="C524" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="525" spans="1:3">
@@ -7701,7 +7695,7 @@
         <v>522</v>
       </c>
       <c r="C525" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="526" spans="1:3">
@@ -7712,7 +7706,7 @@
         <v>523</v>
       </c>
       <c r="C526" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
     </row>
     <row r="527" spans="1:3">
@@ -7723,7 +7717,7 @@
         <v>524</v>
       </c>
       <c r="C527" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
     </row>
     <row r="528" spans="1:3">
@@ -7734,7 +7728,7 @@
         <v>525</v>
       </c>
       <c r="C528" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
     </row>
     <row r="529" spans="1:3">
@@ -7745,7 +7739,7 @@
         <v>526</v>
       </c>
       <c r="C529" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
     </row>
     <row r="530" spans="1:3">
@@ -7756,7 +7750,7 @@
         <v>527</v>
       </c>
       <c r="C530" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
     </row>
   </sheetData>

</xml_diff>